<commit_message>
accidentally update spreadsheet of data
</commit_message>
<xml_diff>
--- a/PizzaParty/input/pizzaparty-small.xlsx
+++ b/PizzaParty/input/pizzaparty-small.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambowker/Desktop/DominosData/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambowker/git/pizzaparty/PizzaParty/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>